<commit_message>
Add new output files
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-measurement-quality.xlsx
+++ b/output/StructureDefinition-measurement-quality.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-26T11:41:10+00:00</t>
+    <t>2024-12-27T22:28:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Indicates the quality and reliability of the measurement</t>
+    <t>Indicator of the quality and reliability of the measurement</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>